<commit_message>
scrum backlog and burndown updated
</commit_message>
<xml_diff>
--- a/SCRUM_backlog.xlsx
+++ b/SCRUM_backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,15 +463,18 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$6:$J$7</c:f>
+              <c:f>Sheet1!$J$6:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0</c:v>
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -486,11 +489,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2125278360"/>
-        <c:axId val="-2135297672"/>
+        <c:axId val="2093923752"/>
+        <c:axId val="2093933656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125278360"/>
+        <c:axId val="2093923752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,7 +522,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135297672"/>
+        <c:crossAx val="2093933656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -527,7 +530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2135297672"/>
+        <c:axId val="2093933656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125278360"/>
+        <c:crossAx val="2093923752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -628,21 +631,6 @@
         <row r="5">
           <cell r="L5" t="str">
             <v>Tasks Left</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="L6">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="L7">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="L8">
-            <v>3</v>
           </cell>
         </row>
       </sheetData>
@@ -980,7 +968,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1078,7 +1066,7 @@
         <v>2</v>
       </c>
       <c r="J7" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1097,6 +1085,9 @@
       <c r="I8" s="5">
         <v>3</v>
       </c>
+      <c r="J8" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="4">
@@ -1176,7 +1167,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -1190,7 +1181,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -1204,7 +1195,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -1218,7 +1209,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
@@ -1234,7 +1225,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D18" s="4">
         <v>2</v>

</xml_diff>

<commit_message>
updated backlog + burndown chart
</commit_message>
<xml_diff>
--- a/SCRUM_backlog.xlsx
+++ b/SCRUM_backlog.xlsx
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Reversi - Product Backlog</t>
   </si>
@@ -431,12 +431,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sprint Burndown Chart - 10/15/13</a:t>
+              <a:t>Sprint Burndown Chart - 10/28/13</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.141936570428696"/>
+          <c:y val="0.00757575757575757"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -463,10 +470,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$6:$J$8</c:f>
+              <c:f>Sheet1!$J$6:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>19.0</c:v>
                 </c:pt>
@@ -475,6 +482,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -489,11 +499,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2093923752"/>
-        <c:axId val="2093933656"/>
+        <c:axId val="2116668168"/>
+        <c:axId val="2090510312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2093923752"/>
+        <c:axId val="2116668168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,7 +532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093933656"/>
+        <c:crossAx val="2090510312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -530,7 +540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2093933656"/>
+        <c:axId val="2090510312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +570,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093923752"/>
+        <c:crossAx val="2116668168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -582,15 +592,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1397000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>2247900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>355600</xdr:rowOff>
+      <xdr:rowOff>520700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -968,7 +978,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1102,6 +1112,12 @@
       <c r="D9" s="4">
         <v>1</v>
       </c>
+      <c r="I9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="4">
@@ -1257,7 +1273,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
@@ -1273,7 +1289,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
@@ -1289,7 +1305,7 @@
         <v>28</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
@@ -1305,7 +1321,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D23" s="4">
         <v>3</v>

</xml_diff>